<commit_message>
0807update - exp about var thickness and data/errorbar
</commit_message>
<xml_diff>
--- a/PycharmCodes_xlsxFiles/var_thick_data18mm.xlsx
+++ b/PycharmCodes_xlsxFiles/var_thick_data18mm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7d89e7b822021c56/Documents/성균관대학교/LAB/skku_robotory/PycharmCodes_xlsxFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{16A6AECC-1355-4078-9F2F-74892DBAF3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7153DAD-B709-4E0B-A931-EDE4C45B4323}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="8_{16A6AECC-1355-4078-9F2F-74892DBAF3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03D06AFD-5490-4568-BBF2-42983D302D38}"/>
   <bookViews>
-    <workbookView xWindow="5076" yWindow="2928" windowWidth="17280" windowHeight="8880" activeTab="6" xr2:uid="{821319C3-96A2-479C-A872-8FF46272A7C1}"/>
+    <workbookView xWindow="864" yWindow="2196" windowWidth="17280" windowHeight="8880" activeTab="6" xr2:uid="{821319C3-96A2-479C-A872-8FF46272A7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="1805" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="1808" sheetId="4" r:id="rId4"/>
     <sheet name="1809" sheetId="5" r:id="rId5"/>
     <sheet name="dn" sheetId="6" r:id="rId6"/>
-    <sheet name="dp" sheetId="7" r:id="rId7"/>
-    <sheet name="un" sheetId="8" r:id="rId8"/>
-    <sheet name="up" sheetId="9" r:id="rId9"/>
+    <sheet name="up" sheetId="9" r:id="rId7"/>
+    <sheet name="dp" sheetId="7" r:id="rId8"/>
+    <sheet name="un" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
   <si>
     <t>10kpa</t>
   </si>
@@ -472,9 +472,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -512,7 +512,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -618,7 +618,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -760,7 +760,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -771,7 +771,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M8"/>
+      <selection activeCell="M8" sqref="K1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -823,22 +823,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>2.08</v>
+        <v>1.25</v>
       </c>
       <c r="C2" s="6">
-        <v>1.8</v>
+        <v>1.27</v>
       </c>
       <c r="D2" s="6">
-        <v>1.75</v>
+        <v>1.31</v>
       </c>
       <c r="E2" s="7">
-        <v>0.88</v>
+        <v>0.98</v>
       </c>
       <c r="F2" s="7">
-        <v>0.88</v>
+        <v>1.29</v>
       </c>
       <c r="G2" s="7">
-        <v>0.73</v>
+        <v>0.89</v>
       </c>
       <c r="H2" s="8">
         <v>2.2999999999999998</v>
@@ -853,10 +853,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="L2" s="9">
-        <v>0.92</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M2" s="9">
-        <v>0.92</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -864,22 +864,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>3.44</v>
+        <v>2.52</v>
       </c>
       <c r="C3" s="6">
-        <v>3.18</v>
+        <v>2.52</v>
       </c>
       <c r="D3" s="6">
-        <v>3.1</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E3" s="7">
-        <v>1.77</v>
+        <v>2.21</v>
       </c>
       <c r="F3" s="7">
-        <v>1.94</v>
+        <v>2.13</v>
       </c>
       <c r="G3" s="7">
-        <v>2.11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H3" s="8">
         <v>4.6900000000000004</v>
@@ -894,10 +894,10 @@
         <v>2.02</v>
       </c>
       <c r="L3" s="9">
-        <v>1.76</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="M3" s="9">
-        <v>1.75</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
@@ -905,22 +905,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>4.59</v>
+        <v>3.65</v>
       </c>
       <c r="C4" s="6">
-        <v>4.3099999999999996</v>
+        <v>3.67</v>
       </c>
       <c r="D4" s="6">
-        <v>4.2</v>
+        <v>3.69</v>
       </c>
       <c r="E4" s="7">
-        <v>3.31</v>
+        <v>3.32</v>
       </c>
       <c r="F4" s="7">
-        <v>3.54</v>
+        <v>3.32</v>
       </c>
       <c r="G4" s="7">
-        <v>3.78</v>
+        <v>3.43</v>
       </c>
       <c r="H4" s="8">
         <v>7.09</v>
@@ -935,10 +935,10 @@
         <v>2.86</v>
       </c>
       <c r="L4" s="9">
-        <v>2.69</v>
+        <v>2.88</v>
       </c>
       <c r="M4" s="9">
-        <v>2.58</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -946,22 +946,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>5.61</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="C5" s="6">
-        <v>5.32</v>
+        <v>4.71</v>
       </c>
       <c r="D5" s="6">
-        <v>5.22</v>
+        <v>4.74</v>
       </c>
       <c r="E5" s="7">
-        <v>4.72</v>
+        <v>4.51</v>
       </c>
       <c r="F5" s="7">
-        <v>4.8499999999999996</v>
+        <v>4.8899999999999997</v>
       </c>
       <c r="G5" s="7">
-        <v>5.32</v>
+        <v>5.05</v>
       </c>
       <c r="H5" s="8">
         <v>9.52</v>
@@ -976,10 +976,10 @@
         <v>3.69</v>
       </c>
       <c r="L5" s="9">
-        <v>3.43</v>
+        <v>3.71</v>
       </c>
       <c r="M5" s="9">
-        <v>3.4</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -987,22 +987,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>6.58</v>
+        <v>5.61</v>
       </c>
       <c r="C6" s="6">
-        <v>6.35</v>
+        <v>5.66</v>
       </c>
       <c r="D6" s="6">
-        <v>6.24</v>
+        <v>5.69</v>
       </c>
       <c r="E6" s="7">
-        <v>6.22</v>
+        <v>6.21</v>
       </c>
       <c r="F6" s="7">
         <v>6.39</v>
       </c>
       <c r="G6" s="7">
-        <v>6.81</v>
+        <v>6.61</v>
       </c>
       <c r="H6" s="8">
         <v>11.88</v>
@@ -1017,10 +1017,10 @@
         <v>4.5</v>
       </c>
       <c r="L6" s="9">
-        <v>4.2300000000000004</v>
+        <v>4.46</v>
       </c>
       <c r="M6" s="9">
-        <v>4.21</v>
+        <v>4.6100000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -1046,10 +1046,10 @@
         <v>5.31</v>
       </c>
       <c r="L7" s="9">
-        <v>5.05</v>
+        <v>5.34</v>
       </c>
       <c r="M7" s="9">
-        <v>5.03</v>
+        <v>5.33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -1075,10 +1075,10 @@
         <v>6.13</v>
       </c>
       <c r="L8" s="9">
-        <v>5.88</v>
+        <v>6.15</v>
       </c>
       <c r="M8" s="9">
-        <v>5.83</v>
+        <v>6.22</v>
       </c>
     </row>
   </sheetData>
@@ -1092,7 +1092,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M8"/>
+      <selection activeCell="E1" sqref="E1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1140,6 +1140,24 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>1.35</v>
+      </c>
+      <c r="C2">
+        <v>1.63</v>
+      </c>
+      <c r="D2">
+        <v>1.82</v>
+      </c>
+      <c r="E2">
+        <v>0.85</v>
+      </c>
+      <c r="F2">
+        <v>0.86</v>
+      </c>
+      <c r="G2">
+        <v>0.83</v>
+      </c>
       <c r="H2" s="10">
         <v>1.37</v>
       </c>
@@ -1163,6 +1181,24 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>2.62</v>
+      </c>
+      <c r="C3">
+        <v>2.81</v>
+      </c>
+      <c r="D3">
+        <v>3.01</v>
+      </c>
+      <c r="E3">
+        <v>1.63</v>
+      </c>
+      <c r="F3">
+        <v>1.82</v>
+      </c>
+      <c r="G3">
+        <v>1.59</v>
+      </c>
       <c r="H3" s="10">
         <v>2.89</v>
       </c>
@@ -1186,6 +1222,24 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>3.88</v>
+      </c>
+      <c r="C4">
+        <v>4.07</v>
+      </c>
+      <c r="D4">
+        <v>4.25</v>
+      </c>
+      <c r="E4">
+        <v>2.38</v>
+      </c>
+      <c r="F4">
+        <v>2.48</v>
+      </c>
+      <c r="G4">
+        <v>2.33</v>
+      </c>
       <c r="H4" s="10">
         <v>4.54</v>
       </c>
@@ -1209,6 +1263,24 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>5.16</v>
+      </c>
+      <c r="C5">
+        <v>5.29</v>
+      </c>
+      <c r="D5">
+        <v>5.47</v>
+      </c>
+      <c r="E5">
+        <v>3.46</v>
+      </c>
+      <c r="F5">
+        <v>3.64</v>
+      </c>
+      <c r="G5">
+        <v>3.62</v>
+      </c>
       <c r="H5" s="10">
         <v>6.77</v>
       </c>
@@ -1231,6 +1303,24 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6.25</v>
+      </c>
+      <c r="C6">
+        <v>6.44</v>
+      </c>
+      <c r="D6">
+        <v>6.39</v>
+      </c>
+      <c r="E6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F6">
+        <v>4.88</v>
+      </c>
+      <c r="G6">
+        <v>4.7300000000000004</v>
       </c>
       <c r="H6" s="10">
         <v>9.08</v>
@@ -1308,7 +1398,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M8"/>
+      <selection activeCell="E1" sqref="E1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1356,6 +1446,24 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2.17</v>
+      </c>
+      <c r="D2">
+        <v>2.35</v>
+      </c>
+      <c r="E2">
+        <v>0.82</v>
+      </c>
+      <c r="F2">
+        <v>0.84</v>
+      </c>
+      <c r="G2">
+        <v>0.62</v>
+      </c>
       <c r="H2" s="10">
         <v>0.68</v>
       </c>
@@ -1379,6 +1487,24 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>3.13</v>
+      </c>
+      <c r="C3">
+        <v>3.33</v>
+      </c>
+      <c r="D3">
+        <v>3.5</v>
+      </c>
+      <c r="E3">
+        <v>1.64</v>
+      </c>
+      <c r="F3">
+        <v>1.33</v>
+      </c>
+      <c r="G3">
+        <v>1.38</v>
+      </c>
       <c r="H3" s="10">
         <v>2.41</v>
       </c>
@@ -1402,6 +1528,24 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>4.25</v>
+      </c>
+      <c r="C4">
+        <v>4.43</v>
+      </c>
+      <c r="D4">
+        <v>4.59</v>
+      </c>
+      <c r="E4">
+        <v>2.39</v>
+      </c>
+      <c r="F4">
+        <v>2.23</v>
+      </c>
+      <c r="G4">
+        <v>2.19</v>
+      </c>
       <c r="H4" s="10">
         <v>4.09</v>
       </c>
@@ -1425,6 +1569,24 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>5.39</v>
+      </c>
+      <c r="C5">
+        <v>5.55</v>
+      </c>
+      <c r="D5">
+        <v>5.67</v>
+      </c>
+      <c r="E5">
+        <v>3.01</v>
+      </c>
+      <c r="F5">
+        <v>2.85</v>
+      </c>
+      <c r="G5">
+        <v>2.92</v>
+      </c>
       <c r="H5" s="10">
         <v>6.06</v>
       </c>
@@ -1447,6 +1609,24 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6.51</v>
+      </c>
+      <c r="C6">
+        <v>6.44</v>
+      </c>
+      <c r="D6">
+        <v>6.55</v>
+      </c>
+      <c r="E6">
+        <v>3.52</v>
+      </c>
+      <c r="F6">
+        <v>3.56</v>
+      </c>
+      <c r="G6">
+        <v>3.52</v>
       </c>
       <c r="H6" s="10">
         <v>8.39</v>
@@ -1524,7 +1704,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M8"/>
+      <selection activeCell="E1" sqref="E1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1572,6 +1752,24 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C2">
+        <v>1.98</v>
+      </c>
+      <c r="D2">
+        <v>1.79</v>
+      </c>
+      <c r="E2">
+        <v>0.85</v>
+      </c>
+      <c r="F2">
+        <v>0.83</v>
+      </c>
+      <c r="G2">
+        <v>0.86</v>
+      </c>
       <c r="H2" s="10">
         <v>1.31</v>
       </c>
@@ -1595,6 +1793,24 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>3.31</v>
+      </c>
+      <c r="C3">
+        <v>3.05</v>
+      </c>
+      <c r="D3">
+        <v>3.12</v>
+      </c>
+      <c r="E3">
+        <v>1.7</v>
+      </c>
+      <c r="F3">
+        <v>1.69</v>
+      </c>
+      <c r="G3">
+        <v>1.67</v>
+      </c>
       <c r="H3" s="10">
         <v>2.63</v>
       </c>
@@ -1618,6 +1834,24 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>4.47</v>
+      </c>
+      <c r="C4">
+        <v>4.21</v>
+      </c>
+      <c r="D4">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E4">
+        <v>2.34</v>
+      </c>
+      <c r="F4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G4">
+        <v>2.31</v>
+      </c>
       <c r="H4" s="10">
         <v>4.5</v>
       </c>
@@ -1641,6 +1875,24 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>5.63</v>
+      </c>
+      <c r="C5">
+        <v>5.41</v>
+      </c>
+      <c r="D5">
+        <v>5.21</v>
+      </c>
+      <c r="E5">
+        <v>2.91</v>
+      </c>
+      <c r="F5">
+        <v>2.85</v>
+      </c>
+      <c r="G5">
+        <v>2.77</v>
+      </c>
       <c r="H5" s="10">
         <v>6.77</v>
       </c>
@@ -1663,6 +1915,24 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6.51</v>
+      </c>
+      <c r="C6">
+        <v>6.62</v>
+      </c>
+      <c r="D6">
+        <v>6.33</v>
+      </c>
+      <c r="E6">
+        <v>3.51</v>
+      </c>
+      <c r="F6">
+        <v>3.71</v>
+      </c>
+      <c r="G6">
+        <v>3.6</v>
       </c>
       <c r="H6" s="10">
         <v>9.23</v>
@@ -1739,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CE86C5-876C-4F30-AFBC-2A3A7FD5A36E}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="E1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1788,6 +2058,24 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>1.38</v>
+      </c>
+      <c r="C2">
+        <v>1.31</v>
+      </c>
+      <c r="D2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E2">
+        <v>1.06</v>
+      </c>
+      <c r="F2">
+        <v>1.26</v>
+      </c>
+      <c r="G2">
+        <v>1.3</v>
+      </c>
       <c r="H2" s="10">
         <v>1.0900000000000001</v>
       </c>
@@ -1811,6 +2099,24 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>2.39</v>
+      </c>
+      <c r="C3">
+        <v>2.31</v>
+      </c>
+      <c r="D3">
+        <v>2.15</v>
+      </c>
+      <c r="E3">
+        <v>2.11</v>
+      </c>
+      <c r="F3">
+        <v>2.29</v>
+      </c>
+      <c r="G3">
+        <v>2.2400000000000002</v>
+      </c>
       <c r="H3" s="10">
         <v>2.39</v>
       </c>
@@ -1834,6 +2140,24 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>3.44</v>
+      </c>
+      <c r="C4">
+        <v>3.36</v>
+      </c>
+      <c r="D4">
+        <v>3.23</v>
+      </c>
+      <c r="E4">
+        <v>3.23</v>
+      </c>
+      <c r="F4">
+        <v>3.38</v>
+      </c>
+      <c r="G4">
+        <v>3.43</v>
+      </c>
       <c r="H4" s="10">
         <v>4.01</v>
       </c>
@@ -1857,6 +2181,24 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="C5">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D5">
+        <v>4.33</v>
+      </c>
+      <c r="E5">
+        <v>4.3</v>
+      </c>
+      <c r="F5">
+        <v>4.53</v>
+      </c>
+      <c r="G5">
+        <v>4.57</v>
+      </c>
       <c r="H5" s="10">
         <v>6.11</v>
       </c>
@@ -1879,6 +2221,24 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5.38</v>
+      </c>
+      <c r="C6">
+        <v>5.49</v>
+      </c>
+      <c r="D6">
+        <v>5.42</v>
+      </c>
+      <c r="E6">
+        <v>5.59</v>
+      </c>
+      <c r="F6">
+        <v>5.65</v>
+      </c>
+      <c r="G6">
+        <v>5.48</v>
       </c>
       <c r="H6" s="10">
         <v>8.4700000000000006</v>
@@ -1953,15 +2313,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1560966-5829-4FAC-B9B6-48D2296A62A4}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D6"/>
+      <selection activeCell="N1" sqref="N1:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -1972,83 +2332,299 @@
       <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>2.08</v>
+        <v>1.25</v>
       </c>
       <c r="C2" s="6">
-        <v>1.8</v>
+        <v>1.27</v>
       </c>
       <c r="D2" s="6">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>1.31</v>
+      </c>
+      <c r="E2">
+        <v>1.35</v>
+      </c>
+      <c r="F2">
+        <v>1.63</v>
+      </c>
+      <c r="G2">
+        <v>1.82</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2.17</v>
+      </c>
+      <c r="J2">
+        <v>2.35</v>
+      </c>
+      <c r="K2">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="L2">
+        <v>1.98</v>
+      </c>
+      <c r="M2">
+        <v>1.79</v>
+      </c>
+      <c r="N2">
+        <v>1.38</v>
+      </c>
+      <c r="O2">
+        <v>1.31</v>
+      </c>
+      <c r="P2">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>3.44</v>
+        <v>2.52</v>
       </c>
       <c r="C3" s="6">
-        <v>3.18</v>
+        <v>2.52</v>
       </c>
       <c r="D3" s="6">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E3">
+        <v>2.62</v>
+      </c>
+      <c r="F3">
+        <v>2.81</v>
+      </c>
+      <c r="G3">
+        <v>3.01</v>
+      </c>
+      <c r="H3">
+        <v>3.13</v>
+      </c>
+      <c r="I3">
+        <v>3.33</v>
+      </c>
+      <c r="J3">
+        <v>3.5</v>
+      </c>
+      <c r="K3">
+        <v>3.31</v>
+      </c>
+      <c r="L3">
+        <v>3.05</v>
+      </c>
+      <c r="M3">
+        <v>3.12</v>
+      </c>
+      <c r="N3">
+        <v>2.39</v>
+      </c>
+      <c r="O3">
+        <v>2.31</v>
+      </c>
+      <c r="P3">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6">
+        <v>3.65</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.67</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3.69</v>
+      </c>
+      <c r="E4">
+        <v>3.88</v>
+      </c>
+      <c r="F4">
+        <v>4.07</v>
+      </c>
+      <c r="G4">
+        <v>4.25</v>
+      </c>
+      <c r="H4">
+        <v>4.25</v>
+      </c>
+      <c r="I4">
+        <v>4.43</v>
+      </c>
+      <c r="J4">
         <v>4.59</v>
       </c>
-      <c r="C4" s="6">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>4.47</v>
+      </c>
+      <c r="L4">
+        <v>4.21</v>
+      </c>
+      <c r="M4">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="N4">
+        <v>3.44</v>
+      </c>
+      <c r="O4">
+        <v>3.36</v>
+      </c>
+      <c r="P4">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>5.61</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="C5" s="6">
-        <v>5.32</v>
+        <v>4.71</v>
       </c>
       <c r="D5" s="6">
-        <v>5.22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>4.74</v>
+      </c>
+      <c r="E5">
+        <v>5.16</v>
+      </c>
+      <c r="F5">
+        <v>5.29</v>
+      </c>
+      <c r="G5">
+        <v>5.47</v>
+      </c>
+      <c r="H5">
+        <v>5.39</v>
+      </c>
+      <c r="I5">
+        <v>5.55</v>
+      </c>
+      <c r="J5">
+        <v>5.67</v>
+      </c>
+      <c r="K5">
+        <v>5.63</v>
+      </c>
+      <c r="L5">
+        <v>5.41</v>
+      </c>
+      <c r="M5">
+        <v>5.21</v>
+      </c>
+      <c r="N5">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="O5">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="P5">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>6.58</v>
+        <v>5.61</v>
       </c>
       <c r="C6" s="6">
-        <v>6.35</v>
+        <v>5.66</v>
       </c>
       <c r="D6" s="6">
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>5.69</v>
+      </c>
+      <c r="E6">
+        <v>6.25</v>
+      </c>
+      <c r="F6">
+        <v>6.44</v>
+      </c>
+      <c r="G6">
+        <v>6.39</v>
+      </c>
+      <c r="H6">
+        <v>6.51</v>
+      </c>
+      <c r="I6">
+        <v>6.44</v>
+      </c>
+      <c r="J6">
+        <v>6.55</v>
+      </c>
+      <c r="K6">
+        <v>6.51</v>
+      </c>
+      <c r="L6">
+        <v>6.62</v>
+      </c>
+      <c r="M6">
+        <v>6.33</v>
+      </c>
+      <c r="N6">
+        <v>5.38</v>
+      </c>
+      <c r="O6">
+        <v>5.49</v>
+      </c>
+      <c r="P6">
+        <v>5.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2060,11 +2636,425 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C260E4E-33F2-4AE2-AFA9-C14BB089B91D}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1.17</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1.08</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1.06</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1.03</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.97</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.97</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.81</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0.68</v>
+      </c>
+      <c r="O2" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2.02</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1.99</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1.91</v>
+      </c>
+      <c r="G3" s="10">
+        <v>1.88</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1.79</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1.79</v>
+      </c>
+      <c r="K3" s="10">
+        <v>1.59</v>
+      </c>
+      <c r="L3" s="10">
+        <v>1.65</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1.64</v>
+      </c>
+      <c r="N3" s="10">
+        <v>1.35</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1.39</v>
+      </c>
+      <c r="P3" s="10">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2.86</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2.88</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2.88</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2.85</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2.76</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="H4" s="10">
+        <v>2.63</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2.63</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2.63</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="L4" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="N4" s="10">
+        <v>2.09</v>
+      </c>
+      <c r="O4" s="10">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="P4" s="10">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3.69</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.71</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3.77</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3.75</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3.61</v>
+      </c>
+      <c r="G5" s="10">
+        <v>3.66</v>
+      </c>
+      <c r="H5" s="10">
+        <v>3.47</v>
+      </c>
+      <c r="I5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="J5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="K5" s="10">
+        <v>3.36</v>
+      </c>
+      <c r="L5" s="10">
+        <v>3.38</v>
+      </c>
+      <c r="M5" s="10">
+        <v>3.38</v>
+      </c>
+      <c r="N5" s="10">
+        <v>2.82</v>
+      </c>
+      <c r="O5" s="10">
+        <v>2.78</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4.46</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E6" s="10">
+        <v>4.55</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4.33</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4.37</v>
+      </c>
+      <c r="H6" s="10">
+        <v>4.34</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4.34</v>
+      </c>
+      <c r="J6" s="10">
+        <v>4.34</v>
+      </c>
+      <c r="K6" s="10">
+        <v>4.25</v>
+      </c>
+      <c r="L6" s="10">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="M6" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="N6" s="10">
+        <v>3.53</v>
+      </c>
+      <c r="O6" s="10">
+        <v>3.55</v>
+      </c>
+      <c r="P6" s="10">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5.31</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5.34</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5.33</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5.41</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5.22</v>
+      </c>
+      <c r="G7" s="10">
+        <v>5.19</v>
+      </c>
+      <c r="H7" s="10">
+        <v>5.18</v>
+      </c>
+      <c r="I7" s="10">
+        <v>5.17</v>
+      </c>
+      <c r="J7" s="10">
+        <v>5.16</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="L7" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="M7" s="10">
+        <v>5.19</v>
+      </c>
+      <c r="N7" s="10">
+        <v>4.26</v>
+      </c>
+      <c r="O7" s="10">
+        <v>4.33</v>
+      </c>
+      <c r="P7" s="10">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>6.13</v>
+      </c>
+      <c r="C8" s="9">
+        <v>6.15</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6.22</v>
+      </c>
+      <c r="E8" s="10">
+        <v>6.07</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6.02</v>
+      </c>
+      <c r="G8" s="10">
+        <v>6.01</v>
+      </c>
+      <c r="H8" s="10">
+        <v>5.9</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5.96</v>
+      </c>
+      <c r="J8" s="10">
+        <v>6</v>
+      </c>
+      <c r="K8" s="10">
+        <v>6.04</v>
+      </c>
+      <c r="L8" s="10">
+        <v>6.04</v>
+      </c>
+      <c r="M8" s="10">
+        <v>6.07</v>
+      </c>
+      <c r="N8" s="10">
+        <v>5.03</v>
+      </c>
+      <c r="O8" s="10">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="P8" s="10">
+        <v>5.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FB809B-D272-408F-A56F-B50250C1B8A7}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2529,520 +3519,322 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247121A8-E4D5-4E11-907B-BF9DEE51D368}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="C2" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1.77</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1.94</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3.31</v>
-      </c>
-      <c r="C4" s="7">
-        <v>3.54</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7">
-        <v>4.72</v>
-      </c>
-      <c r="C5" s="7">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="D5" s="7">
-        <v>5.32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <v>6.22</v>
-      </c>
-      <c r="C6" s="7">
-        <v>6.39</v>
-      </c>
-      <c r="D6" s="7">
-        <v>6.81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C260E4E-33F2-4AE2-AFA9-C14BB089B91D}">
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:P8"/>
+      <selection activeCell="P6" sqref="N1:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>64</v>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0.92</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.92</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1.08</v>
-      </c>
-      <c r="F2" s="10">
+      <c r="B2" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.29</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="E2">
+        <v>0.85</v>
+      </c>
+      <c r="F2">
+        <v>0.86</v>
+      </c>
+      <c r="G2">
+        <v>0.83</v>
+      </c>
+      <c r="H2">
+        <v>0.82</v>
+      </c>
+      <c r="I2">
+        <v>0.84</v>
+      </c>
+      <c r="J2">
+        <v>0.62</v>
+      </c>
+      <c r="K2">
+        <v>0.85</v>
+      </c>
+      <c r="L2">
+        <v>0.83</v>
+      </c>
+      <c r="M2">
+        <v>0.86</v>
+      </c>
+      <c r="N2">
         <v>1.06</v>
       </c>
-      <c r="G2" s="10">
-        <v>1.03</v>
-      </c>
-      <c r="H2" s="10">
-        <v>0.93</v>
-      </c>
-      <c r="I2" s="10">
-        <v>0.97</v>
-      </c>
-      <c r="J2" s="10">
-        <v>0.97</v>
-      </c>
-      <c r="K2" s="10">
-        <v>0.81</v>
-      </c>
-      <c r="L2" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="M2" s="10">
-        <v>0.87</v>
-      </c>
-      <c r="N2" s="10">
-        <v>0.68</v>
-      </c>
-      <c r="O2" s="10">
-        <v>0.69</v>
-      </c>
-      <c r="P2" s="10">
-        <v>0.57999999999999996</v>
+      <c r="O2">
+        <v>1.26</v>
+      </c>
+      <c r="P2">
+        <v>1.3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>2.02</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1.76</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1.99</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1.91</v>
-      </c>
-      <c r="G3" s="10">
-        <v>1.88</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1.79</v>
-      </c>
-      <c r="I3" s="10">
-        <v>1.8</v>
-      </c>
-      <c r="J3" s="10">
-        <v>1.79</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="B3" s="7">
+        <v>2.21</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2.13</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E3">
+        <v>1.63</v>
+      </c>
+      <c r="F3">
+        <v>1.82</v>
+      </c>
+      <c r="G3">
         <v>1.59</v>
       </c>
-      <c r="L3" s="10">
-        <v>1.65</v>
-      </c>
-      <c r="M3" s="10">
+      <c r="H3">
         <v>1.64</v>
       </c>
-      <c r="N3" s="10">
-        <v>1.35</v>
-      </c>
-      <c r="O3" s="10">
-        <v>1.39</v>
-      </c>
-      <c r="P3" s="10">
-        <v>1.36</v>
+      <c r="I3">
+        <v>1.33</v>
+      </c>
+      <c r="J3">
+        <v>1.38</v>
+      </c>
+      <c r="K3">
+        <v>1.7</v>
+      </c>
+      <c r="L3">
+        <v>1.69</v>
+      </c>
+      <c r="M3">
+        <v>1.67</v>
+      </c>
+      <c r="N3">
+        <v>2.11</v>
+      </c>
+      <c r="O3">
+        <v>2.29</v>
+      </c>
+      <c r="P3">
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
-        <v>2.86</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2.69</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2.58</v>
-      </c>
-      <c r="E4" s="10">
-        <v>2.85</v>
-      </c>
-      <c r="F4" s="10">
-        <v>2.76</v>
-      </c>
-      <c r="G4" s="10">
-        <v>2.75</v>
-      </c>
-      <c r="H4" s="10">
-        <v>2.63</v>
-      </c>
-      <c r="I4" s="10">
-        <v>2.63</v>
-      </c>
-      <c r="J4" s="10">
-        <v>2.63</v>
-      </c>
-      <c r="K4" s="10">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="L4" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="M4" s="10">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="N4" s="10">
-        <v>2.09</v>
-      </c>
-      <c r="O4" s="10">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="P4" s="10">
-        <v>2.0299999999999998</v>
+      <c r="B4" s="7">
+        <v>3.32</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3.32</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3.43</v>
+      </c>
+      <c r="E4">
+        <v>2.38</v>
+      </c>
+      <c r="F4">
+        <v>2.48</v>
+      </c>
+      <c r="G4">
+        <v>2.33</v>
+      </c>
+      <c r="H4">
+        <v>2.39</v>
+      </c>
+      <c r="I4">
+        <v>2.23</v>
+      </c>
+      <c r="J4">
+        <v>2.19</v>
+      </c>
+      <c r="K4">
+        <v>2.34</v>
+      </c>
+      <c r="L4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="M4">
+        <v>2.31</v>
+      </c>
+      <c r="N4">
+        <v>3.23</v>
+      </c>
+      <c r="O4">
+        <v>3.38</v>
+      </c>
+      <c r="P4">
+        <v>3.43</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
-        <v>3.69</v>
-      </c>
-      <c r="C5" s="9">
-        <v>3.43</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3.4</v>
-      </c>
-      <c r="E5" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="F5" s="10">
-        <v>3.61</v>
-      </c>
-      <c r="G5" s="10">
-        <v>3.66</v>
-      </c>
-      <c r="H5" s="10">
-        <v>3.47</v>
-      </c>
-      <c r="I5" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="J5" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="K5" s="10">
-        <v>3.36</v>
-      </c>
-      <c r="L5" s="10">
-        <v>3.38</v>
-      </c>
-      <c r="M5" s="10">
-        <v>3.38</v>
-      </c>
-      <c r="N5" s="10">
-        <v>2.82</v>
-      </c>
-      <c r="O5" s="10">
-        <v>2.78</v>
-      </c>
-      <c r="P5" s="10">
-        <v>2.81</v>
+      <c r="B5" s="7">
+        <v>4.51</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5.05</v>
+      </c>
+      <c r="E5">
+        <v>3.46</v>
+      </c>
+      <c r="F5">
+        <v>3.64</v>
+      </c>
+      <c r="G5">
+        <v>3.62</v>
+      </c>
+      <c r="H5">
+        <v>3.01</v>
+      </c>
+      <c r="I5">
+        <v>2.85</v>
+      </c>
+      <c r="J5">
+        <v>2.92</v>
+      </c>
+      <c r="K5">
+        <v>2.91</v>
+      </c>
+      <c r="L5">
+        <v>2.85</v>
+      </c>
+      <c r="M5">
+        <v>2.77</v>
+      </c>
+      <c r="N5">
+        <v>4.3</v>
+      </c>
+      <c r="O5">
+        <v>4.53</v>
+      </c>
+      <c r="P5">
+        <v>4.57</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
-        <v>4.5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4.21</v>
-      </c>
-      <c r="E6" s="10">
-        <v>4.55</v>
-      </c>
-      <c r="F6" s="10">
-        <v>4.33</v>
-      </c>
-      <c r="G6" s="10">
-        <v>4.37</v>
-      </c>
-      <c r="H6" s="10">
-        <v>4.34</v>
-      </c>
-      <c r="I6" s="10">
-        <v>4.34</v>
-      </c>
-      <c r="J6" s="10">
-        <v>4.34</v>
-      </c>
-      <c r="K6" s="10">
-        <v>4.25</v>
-      </c>
-      <c r="L6" s="10">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="M6" s="10">
-        <v>4.3</v>
-      </c>
-      <c r="N6" s="10">
-        <v>3.53</v>
-      </c>
-      <c r="O6" s="10">
-        <v>3.55</v>
-      </c>
-      <c r="P6" s="10">
-        <v>3.58</v>
+      <c r="B6" s="7">
+        <v>6.21</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6.39</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6.61</v>
+      </c>
+      <c r="E6">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F6">
+        <v>4.88</v>
+      </c>
+      <c r="G6">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="H6">
+        <v>3.52</v>
+      </c>
+      <c r="I6">
+        <v>3.56</v>
+      </c>
+      <c r="J6">
+        <v>3.52</v>
+      </c>
+      <c r="K6">
+        <v>3.51</v>
+      </c>
+      <c r="L6">
+        <v>3.71</v>
+      </c>
+      <c r="M6">
+        <v>3.6</v>
+      </c>
+      <c r="N6">
+        <v>5.59</v>
+      </c>
+      <c r="O6">
+        <v>5.65</v>
+      </c>
+      <c r="P6">
+        <v>5.48</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>5.31</v>
-      </c>
-      <c r="C7" s="9">
-        <v>5.05</v>
-      </c>
-      <c r="D7" s="9">
-        <v>5.03</v>
-      </c>
-      <c r="E7" s="10">
-        <v>5.41</v>
-      </c>
-      <c r="F7" s="10">
-        <v>5.22</v>
-      </c>
-      <c r="G7" s="10">
-        <v>5.19</v>
-      </c>
-      <c r="H7" s="10">
-        <v>5.18</v>
-      </c>
-      <c r="I7" s="10">
-        <v>5.17</v>
-      </c>
-      <c r="J7" s="10">
-        <v>5.16</v>
-      </c>
-      <c r="K7" s="10">
-        <v>5.15</v>
-      </c>
-      <c r="L7" s="10">
-        <v>5.15</v>
-      </c>
-      <c r="M7" s="10">
-        <v>5.19</v>
-      </c>
-      <c r="N7" s="10">
-        <v>4.26</v>
-      </c>
-      <c r="O7" s="10">
-        <v>4.33</v>
-      </c>
-      <c r="P7" s="10">
-        <v>4.3499999999999996</v>
-      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="9">
-        <v>6.13</v>
-      </c>
-      <c r="C8" s="9">
-        <v>5.88</v>
-      </c>
-      <c r="D8" s="9">
-        <v>5.83</v>
-      </c>
-      <c r="E8" s="10">
-        <v>6.07</v>
-      </c>
-      <c r="F8" s="10">
-        <v>6.02</v>
-      </c>
-      <c r="G8" s="10">
-        <v>6.01</v>
-      </c>
-      <c r="H8" s="10">
-        <v>5.9</v>
-      </c>
-      <c r="I8" s="10">
-        <v>5.96</v>
-      </c>
-      <c r="J8" s="10">
-        <v>6</v>
-      </c>
-      <c r="K8" s="10">
-        <v>6.04</v>
-      </c>
-      <c r="L8" s="10">
-        <v>6.04</v>
-      </c>
-      <c r="M8" s="10">
-        <v>6.07</v>
-      </c>
-      <c r="N8" s="10">
-        <v>5.03</v>
-      </c>
-      <c r="O8" s="10">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="P8" s="10">
-        <v>5.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>